<commit_message>
trying to make r scripts reproducible
</commit_message>
<xml_diff>
--- a/code/RTMR_Output/Keywords/Keywords_Regions_freq.xlsx
+++ b/code/RTMR_Output/Keywords/Keywords_Regions_freq.xlsx
@@ -581,7 +581,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>libya</t>
+          <t>vietnam</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -591,7 +591,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>vietnam</t>
+          <t>libya</t>
         </is>
       </c>
       <c r="B17" t="n">

</xml_diff>

<commit_message>
clean, annotate, and rerun code
</commit_message>
<xml_diff>
--- a/code/RTMR_Output/Keywords/Keywords_Regions_freq.xlsx
+++ b/code/RTMR_Output/Keywords/Keywords_Regions_freq.xlsx
@@ -581,7 +581,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>libya</t>
+          <t>vietnam</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -591,7 +591,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>vietnam</t>
+          <t>libya</t>
         </is>
       </c>
       <c r="B17" t="n">

</xml_diff>